<commit_message>
Added EDSM data, modified task tracking
</commit_message>
<xml_diff>
--- a/PelagicSurveys_AnalysisTaskTracking.xlsx
+++ b/PelagicSurveys_AnalysisTaskTracking.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40545\ICF\IEP Fish Survey Evaluation - General\Survey Evaluation and Design - Shared\Public\4. Workplan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40545\Documents\GitHub\pelagicsurveys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73898A30-488A-4134-ADEA-3371D0552C30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2D40DD-0229-4E86-98A8-13E3EA36B2A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19290" yWindow="-5320" windowWidth="19380" windowHeight="10380" xr2:uid="{7A9AC542-BDC1-4323-B5A2-F1D810EC1444}"/>
   </bookViews>
@@ -30,6 +30,200 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="63">
+  <si>
+    <t>Analysis Group</t>
+  </si>
+  <si>
+    <t>Regional Abundance Estimates</t>
+  </si>
+  <si>
+    <t>Spatial Distribution of Species</t>
+  </si>
+  <si>
+    <t>Long-Term Trends</t>
+  </si>
+  <si>
+    <t>Sampling Method Optimization</t>
+  </si>
+  <si>
+    <t>Evaluation of Existing Data</t>
+  </si>
+  <si>
+    <t>Analysis Subgroup</t>
+  </si>
+  <si>
+    <t>How are stations distributed across regions, depths and habitats?</t>
+  </si>
+  <si>
+    <t>Primary Survey</t>
+  </si>
+  <si>
+    <t>Secondary Surveys</t>
+  </si>
+  <si>
+    <t>External Surveys</t>
+  </si>
+  <si>
+    <t>FMWT</t>
+  </si>
+  <si>
+    <t>SKT, STN</t>
+  </si>
+  <si>
+    <t>How are stations distributed relative to environmental gradients?</t>
+  </si>
+  <si>
+    <t>Question/ Task</t>
+  </si>
+  <si>
+    <t>Calculate estimates of abundance at Delta sub-regional scales</t>
+  </si>
+  <si>
+    <t>Which stations have least impact on abundance estimates/ uncertainty?</t>
+  </si>
+  <si>
+    <t>Analytical Stage</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Data acquisition and preparation</t>
+  </si>
+  <si>
+    <t>Obtain Survey Data</t>
+  </si>
+  <si>
+    <t>Convert to flat .csv</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Nearing completion</t>
+  </si>
+  <si>
+    <t>STN</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Tillotson</t>
+  </si>
+  <si>
+    <t>SKT</t>
+  </si>
+  <si>
+    <t>20mm</t>
+  </si>
+  <si>
+    <t>SLS</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>EDSM</t>
+  </si>
+  <si>
+    <t>Scheduled Completion</t>
+  </si>
+  <si>
+    <t>NotAssigned</t>
+  </si>
+  <si>
+    <t>Next Steps</t>
+  </si>
+  <si>
+    <t>Index Method</t>
+  </si>
+  <si>
+    <t>Subtask/ Detail</t>
+  </si>
+  <si>
+    <t>GIS</t>
+  </si>
+  <si>
+    <t>Raw Catch</t>
+  </si>
+  <si>
+    <t>Desgin-based estimators</t>
+  </si>
+  <si>
+    <t>Catchability for species other than DS</t>
+  </si>
+  <si>
+    <t>Locate/generate fish catch selection curves</t>
+  </si>
+  <si>
+    <t>Species A</t>
+  </si>
+  <si>
+    <t>Specis B</t>
+  </si>
+  <si>
+    <t>Calculate observed retention probability by length</t>
+  </si>
+  <si>
+    <t>Quantify variation in catchability between species</t>
+  </si>
+  <si>
+    <t>Quantify variation in catchability between surveys</t>
+  </si>
+  <si>
+    <t>Quantify variation in catchability through time</t>
+  </si>
+  <si>
+    <t>Model relationships with covariates</t>
+  </si>
+  <si>
+    <t>Multivariate analysis of spatiotemporal patterns</t>
+  </si>
+  <si>
+    <t>Identify stations with high/low species diversity, catch rates, etc.</t>
+  </si>
+  <si>
+    <t>Generate station rankings based on multiple criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fit temporal trend models </t>
+  </si>
+  <si>
+    <t>Single survey trends</t>
+  </si>
+  <si>
+    <t>Combined survey trends</t>
+  </si>
+  <si>
+    <t>FMWT,STN,SKT</t>
+  </si>
+  <si>
+    <t>Compare trends among regions</t>
+  </si>
+  <si>
+    <t>Explore variability in abundance estimates between regions and years</t>
+  </si>
+  <si>
+    <t>Evaluate the influence of # of tows</t>
+  </si>
+  <si>
+    <t>Evaluate the influence of tow duration</t>
+  </si>
+  <si>
+    <t>Evaluate representativeness of size distributions</t>
+  </si>
+  <si>
+    <t>Initiated</t>
+  </si>
+  <si>
+    <t>Meet with ICF GIS team</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -41,12 +235,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -61,8 +273,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,12 +592,654 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CD1101-A740-442D-9EF8-4D094F36F8EE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" customWidth="1"/>
+    <col min="4" max="4" width="43.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Complete initial data integration
</commit_message>
<xml_diff>
--- a/PelagicSurveys_AnalysisTaskTracking.xlsx
+++ b/PelagicSurveys_AnalysisTaskTracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40545\Documents\GitHub\pelagicsurveys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2D40DD-0229-4E86-98A8-13E3EA36B2A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DE116C-7A80-45B5-9431-456095C9AF53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="-5320" windowWidth="19380" windowHeight="10380" xr2:uid="{7A9AC542-BDC1-4323-B5A2-F1D810EC1444}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A9AC542-BDC1-4323-B5A2-F1D810EC1444}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="64">
   <si>
     <t>Analysis Group</t>
   </si>
@@ -123,18 +123,12 @@
     <t>SLS</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>EDSM</t>
   </si>
   <si>
     <t>Scheduled Completion</t>
   </si>
   <si>
-    <t>NotAssigned</t>
-  </si>
-  <si>
     <t>Next Steps</t>
   </si>
   <si>
@@ -220,6 +214,15 @@
   </si>
   <si>
     <t>Meet with ICF GIS team</t>
+  </si>
+  <si>
+    <t>Gereral</t>
+  </si>
+  <si>
+    <t>Integrate Datasets</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -235,7 +238,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,12 +257,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -273,11 +270,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CD1101-A740-442D-9EF8-4D094F36F8EE}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,7 +619,7 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -641,10 +637,10 @@
         <v>17</v>
       </c>
       <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
         <v>32</v>
-      </c>
-      <c r="K1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -683,8 +679,8 @@
       <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>23</v>
+      <c r="I3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -723,8 +719,8 @@
       <c r="H5" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>23</v>
+      <c r="I5" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -763,8 +759,8 @@
       <c r="H7" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>30</v>
+      <c r="I7" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -781,10 +777,10 @@
         <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -801,10 +797,10 @@
         <v>28</v>
       </c>
       <c r="H9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -821,10 +817,10 @@
         <v>29</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -841,10 +837,10 @@
         <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -858,10 +854,10 @@
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
@@ -881,10 +877,10 @@
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
@@ -895,31 +891,22 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="H14" t="s">
         <v>26</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K14" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -930,7 +917,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -938,6 +928,15 @@
       <c r="F15" t="s">
         <v>12</v>
       </c>
+      <c r="H15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -947,10 +946,13 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -961,16 +963,10 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
-      </c>
-      <c r="F17" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -984,7 +980,7 @@
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -1004,7 +1000,7 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -1018,16 +1014,19 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1035,13 +1034,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
         <v>40</v>
-      </c>
-      <c r="C21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" t="s">
-        <v>43</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1052,10 +1051,16 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1063,10 +1068,10 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1074,10 +1079,10 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1085,10 +1090,10 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1096,10 +1101,10 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1110,7 +1115,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1121,7 +1126,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1132,7 +1137,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1140,16 +1145,10 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1160,13 +1159,13 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1177,10 +1176,13 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
+        <v>52</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1191,7 +1193,7 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
@@ -1202,10 +1204,10 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
@@ -1219,7 +1221,7 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E35" t="s">
         <v>11</v>
@@ -1233,9 +1235,23 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix SKT and 20mm issues, finish wide format spatial data
</commit_message>
<xml_diff>
--- a/PelagicSurveys_AnalysisTaskTracking.xlsx
+++ b/PelagicSurveys_AnalysisTaskTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40545\Documents\GitHub\pelagicsurveys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DE116C-7A80-45B5-9431-456095C9AF53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEDE1B1-2631-42E1-8433-13855C83902A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A9AC542-BDC1-4323-B5A2-F1D810EC1444}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="63">
   <si>
     <t>Analysis Group</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Complete</t>
-  </si>
-  <si>
-    <t>Nearing completion</t>
   </si>
   <si>
     <t>STN</t>
@@ -590,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CD1101-A740-442D-9EF8-4D094F36F8EE}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,7 +616,7 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
         <v>8</v>
@@ -631,16 +628,16 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I1" t="s">
         <v>17</v>
       </c>
       <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
         <v>31</v>
-      </c>
-      <c r="K1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -657,7 +654,7 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>22</v>
@@ -677,7 +674,7 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>22</v>
@@ -694,10 +691,10 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>22</v>
@@ -714,10 +711,10 @@
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>22</v>
@@ -734,10 +731,10 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>22</v>
@@ -754,10 +751,10 @@
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>22</v>
@@ -774,10 +771,10 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>22</v>
@@ -794,10 +791,10 @@
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>22</v>
@@ -814,10 +811,10 @@
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>22</v>
@@ -834,10 +831,10 @@
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>22</v>
@@ -854,13 +851,13 @@
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>22</v>
@@ -877,13 +874,13 @@
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>22</v>
@@ -891,22 +888,22 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
       </c>
       <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
         <v>62</v>
       </c>
-      <c r="E14" t="s">
-        <v>63</v>
-      </c>
       <c r="H14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -920,7 +917,7 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -929,13 +926,13 @@
         <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" t="s">
         <v>59</v>
-      </c>
-      <c r="K15" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -980,7 +977,7 @@
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
@@ -1000,7 +997,7 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -1020,7 +1017,7 @@
         <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
@@ -1034,13 +1031,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
         <v>38</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>39</v>
-      </c>
-      <c r="D21" t="s">
-        <v>40</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1051,13 +1048,13 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
         <v>38</v>
       </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
@@ -1068,10 +1065,10 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1079,10 +1076,10 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1090,10 +1087,10 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1101,10 +1098,10 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1115,7 +1112,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1126,7 +1123,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1137,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1148,7 +1145,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1159,10 +1156,10 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" t="s">
         <v>50</v>
-      </c>
-      <c r="D31" t="s">
-        <v>51</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
@@ -1176,13 +1173,13 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" t="s">
         <v>52</v>
-      </c>
-      <c r="E32" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1193,7 +1190,7 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
@@ -1207,7 +1204,7 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
@@ -1221,7 +1218,7 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E35" t="s">
         <v>11</v>
@@ -1235,7 +1232,7 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
@@ -1249,7 +1246,7 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E37" t="s">
         <v>11</v>

</xml_diff>